<commit_message>
grind sliding window #day2
Signed-off-by: Aditya <aditya@gravityilabs.com>
</commit_message>
<xml_diff>
--- a/coding-Progress.xlsx
+++ b/coding-Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\go-workspace\src\github.com\aditya109\grokking-the-coding-interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCF12BB-B91C-4F1B-8C35-76B6E00E505A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD051E40-F3AB-4896-B100-1523830EC8DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12825" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13335" yWindow="2925" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,6 +286,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,39 +326,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -611,38 +611,38 @@
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="10" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
@@ -658,10 +658,10 @@
       <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -670,16 +670,16 @@
       <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
@@ -687,9 +687,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
         <v>33</v>
@@ -697,7 +695,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
@@ -705,9 +703,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
         <v>33</v>
@@ -715,19 +711,23 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
@@ -739,7 +739,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
@@ -751,7 +751,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="4" t="s">
         <v>32</v>
       </c>
@@ -767,7 +767,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -777,7 +777,7 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -787,7 +787,7 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -797,7 +797,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -807,7 +807,7 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="4"/>
@@ -819,7 +819,7 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -829,7 +829,7 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -839,7 +839,7 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -849,7 +849,7 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="4"/>
@@ -861,7 +861,7 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -871,7 +871,7 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -881,7 +881,7 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -891,7 +891,7 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -901,7 +901,7 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -911,7 +911,7 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -921,7 +921,7 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="4"/>
@@ -933,7 +933,7 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -943,7 +943,7 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -953,7 +953,7 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -963,7 +963,7 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -973,7 +973,7 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -983,7 +983,7 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -993,7 +993,7 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="4"/>
@@ -1005,7 +1005,7 @@
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1015,7 +1015,7 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1025,7 +1025,7 @@
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1035,7 +1035,7 @@
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1045,7 +1045,7 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="4"/>
@@ -1057,7 +1057,7 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="4"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1067,7 +1067,7 @@
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1077,7 +1077,7 @@
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1087,7 +1087,7 @@
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1097,7 +1097,7 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="4"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1107,7 +1107,7 @@
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="4"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1117,7 +1117,7 @@
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="4"/>
@@ -1129,7 +1129,7 @@
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="4"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1139,7 +1139,7 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1149,7 +1149,7 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="4"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1159,7 +1159,7 @@
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1169,7 +1169,7 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="4"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1179,7 +1179,7 @@
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="4"/>
@@ -1191,7 +1191,7 @@
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="4"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -1201,7 +1201,7 @@
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -1211,7 +1211,7 @@
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="4"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -1221,7 +1221,7 @@
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="4"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -1231,7 +1231,7 @@
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="4"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -1241,7 +1241,7 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="4"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -1251,7 +1251,7 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="4"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -1261,7 +1261,7 @@
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B58" s="4"/>
@@ -1273,7 +1273,7 @@
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="4"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -1283,7 +1283,7 @@
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="4"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -1293,7 +1293,7 @@
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
+      <c r="A61" s="11"/>
       <c r="B61" s="4"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -1303,7 +1303,7 @@
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="12"/>
       <c r="B62" s="4"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -1313,7 +1313,7 @@
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B63" s="4"/>
@@ -1325,7 +1325,7 @@
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+      <c r="A64" s="11"/>
       <c r="B64" s="4"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -1335,7 +1335,7 @@
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="4"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -1345,7 +1345,7 @@
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+      <c r="A66" s="11"/>
       <c r="B66" s="4"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -1355,7 +1355,7 @@
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="4"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -1365,7 +1365,7 @@
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="12"/>
       <c r="B68" s="4"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -1375,7 +1375,7 @@
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B69" s="4"/>
@@ -1387,7 +1387,7 @@
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="4"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -1397,7 +1397,7 @@
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+      <c r="A71" s="11"/>
       <c r="B71" s="4"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -1407,7 +1407,7 @@
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
+      <c r="A72" s="11"/>
       <c r="B72" s="4"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -1417,7 +1417,7 @@
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
+      <c r="A73" s="11"/>
       <c r="B73" s="4"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -1427,7 +1427,7 @@
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
+      <c r="A74" s="11"/>
       <c r="B74" s="4"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -1437,7 +1437,7 @@
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="12"/>
       <c r="B75" s="4"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -1447,7 +1447,7 @@
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B76" s="4"/>
@@ -1459,7 +1459,7 @@
       <c r="H76" s="1"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
+      <c r="A77" s="11"/>
       <c r="B77" s="4"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -1469,7 +1469,7 @@
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
+      <c r="A78" s="11"/>
       <c r="B78" s="4"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -1479,7 +1479,7 @@
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
+      <c r="A79" s="11"/>
       <c r="B79" s="4"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -1489,7 +1489,7 @@
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="12"/>
       <c r="B80" s="4"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -1499,7 +1499,7 @@
       <c r="H80" s="1"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
+      <c r="A81" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B81" s="4"/>
@@ -1511,7 +1511,7 @@
       <c r="H81" s="1"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
+      <c r="A82" s="11"/>
       <c r="B82" s="4"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -1521,7 +1521,7 @@
       <c r="H82" s="1"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
+      <c r="A83" s="11"/>
       <c r="B83" s="4"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -1531,7 +1531,7 @@
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
+      <c r="A84" s="11"/>
       <c r="B84" s="4"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -1541,7 +1541,7 @@
       <c r="H84" s="1"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
+      <c r="A85" s="11"/>
       <c r="B85" s="4"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -1551,7 +1551,7 @@
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="13"/>
+      <c r="A86" s="11"/>
       <c r="B86" s="4"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -1561,7 +1561,7 @@
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="13"/>
+      <c r="A87" s="11"/>
       <c r="B87" s="4"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -1571,7 +1571,7 @@
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
+      <c r="A88" s="12"/>
       <c r="B88" s="4"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -1581,7 +1581,7 @@
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B89" s="4"/>
@@ -1593,7 +1593,7 @@
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
+      <c r="A90" s="11"/>
       <c r="B90" s="4"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -1603,7 +1603,7 @@
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
+      <c r="A91" s="11"/>
       <c r="B91" s="4"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -1613,7 +1613,7 @@
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="13"/>
+      <c r="A92" s="11"/>
       <c r="B92" s="4"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
@@ -1623,7 +1623,7 @@
       <c r="H92" s="1"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="13"/>
+      <c r="A93" s="11"/>
       <c r="B93" s="4"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -1633,7 +1633,7 @@
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
+      <c r="A94" s="11"/>
       <c r="B94" s="4"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
@@ -1643,7 +1643,7 @@
       <c r="H94" s="1"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="12"/>
       <c r="B95" s="4"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
@@ -1653,7 +1653,7 @@
       <c r="H95" s="1"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+      <c r="A96" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B96" s="4"/>
@@ -1665,7 +1665,7 @@
       <c r="H96" s="1"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
+      <c r="A97" s="14"/>
       <c r="B97" s="4"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
@@ -1675,7 +1675,7 @@
       <c r="H97" s="1"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
+      <c r="A98" s="14"/>
       <c r="B98" s="4"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -1685,7 +1685,7 @@
       <c r="H98" s="1"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
+      <c r="A99" s="14"/>
       <c r="B99" s="4"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -1695,7 +1695,7 @@
       <c r="H99" s="1"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
+      <c r="A100" s="14"/>
       <c r="B100" s="4"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -1705,7 +1705,7 @@
       <c r="H100" s="1"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
+      <c r="A101" s="14"/>
       <c r="B101" s="4"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
@@ -1715,7 +1715,7 @@
       <c r="H101" s="1"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
+      <c r="A102" s="14"/>
       <c r="B102" s="4"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
@@ -1725,7 +1725,7 @@
       <c r="H102" s="1"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
+      <c r="A103" s="14"/>
       <c r="B103" s="4"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -1735,7 +1735,7 @@
       <c r="H103" s="1"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="18"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="4"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
@@ -1745,7 +1745,7 @@
       <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
+      <c r="A105" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B105" s="4"/>
@@ -1757,7 +1757,7 @@
       <c r="H105" s="1"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="13"/>
+      <c r="A106" s="11"/>
       <c r="B106" s="4"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -1767,7 +1767,7 @@
       <c r="H106" s="1"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
+      <c r="A107" s="12"/>
       <c r="B107" s="4"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -1790,26 +1790,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="A58:A62"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A75"/>
     <mergeCell ref="A76:A80"/>
     <mergeCell ref="A81:A88"/>
     <mergeCell ref="A89:A95"/>
     <mergeCell ref="A96:A104"/>
     <mergeCell ref="A105:A107"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="A63:A68"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A3:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2 pointers grind practice problems completed ;
</commit_message>
<xml_diff>
--- a/coding-Progress.xlsx
+++ b/coding-Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\go-workspace\src\github.com\aditya109\grokking-the-coding-interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F2E66-7C0B-4C52-8D8B-83692583DC0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC5AB5B-4358-43D6-95BE-2D2A5DD3F56C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="2625" windowWidth="21600" windowHeight="11385" tabRatio="251" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="251" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>Problem Pattern</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t xml:space="preserve">                  </t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -421,6 +424,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,10 +457,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -452,24 +473,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -756,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,25 +769,25 @@
     <col min="2" max="2" width="42.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="6"/>
     <col min="7" max="7" width="14.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="14" customWidth="1"/>
     <col min="9" max="9" width="25.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="18" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="24" t="s">
@@ -792,8 +795,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
@@ -806,14 +809,14 @@
       <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="18"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -825,16 +828,16 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
@@ -844,14 +847,14 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="15"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
@@ -861,14 +864,14 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="15"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
@@ -878,14 +881,14 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="15"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
@@ -895,14 +898,14 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="15"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
@@ -912,14 +915,14 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
@@ -929,14 +932,14 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="9" t="s">
         <v>34</v>
       </c>
@@ -946,14 +949,14 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="9" t="s">
         <v>35</v>
       </c>
@@ -963,14 +966,14 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="15"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="9" t="s">
         <v>36</v>
       </c>
@@ -978,12 +981,12 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="9" t="s">
         <v>37</v>
       </c>
@@ -991,34 +994,34 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="15"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="2"/>
@@ -1026,23 +1029,23 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="14"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
@@ -1050,89 +1053,89 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="15"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="15"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="23"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="15"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="23"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="16"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="2"/>
@@ -1140,78 +1143,78 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="14"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="12"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="15"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="23"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="15"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="15"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="23"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="15"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="23"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="15"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="23"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="16"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="2"/>
@@ -1219,78 +1222,78 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="23"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="14"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="23"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="15"/>
+      <c r="I34" s="20"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="23"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="15"/>
+      <c r="I35" s="20"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="23"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="15"/>
+      <c r="I36" s="20"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="23"/>
+      <c r="G37" s="12"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="15"/>
+      <c r="I37" s="20"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="23"/>
+      <c r="G38" s="12"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="15"/>
+      <c r="I38" s="20"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="23"/>
+      <c r="G39" s="12"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="16"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="2"/>
@@ -1298,56 +1301,56 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="23"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="14"/>
+      <c r="I40" s="19"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="23"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="15"/>
+      <c r="I41" s="20"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="23"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="15"/>
+      <c r="I42" s="20"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="23"/>
+      <c r="G43" s="12"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="15"/>
+      <c r="I43" s="20"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="23"/>
+      <c r="G44" s="12"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="16"/>
+      <c r="I44" s="21"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="2"/>
@@ -1355,78 +1358,78 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="23"/>
+      <c r="G45" s="12"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="14"/>
+      <c r="I45" s="19"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="23"/>
+      <c r="G46" s="12"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="15"/>
+      <c r="I46" s="20"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="23"/>
+      <c r="G47" s="12"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="15"/>
+      <c r="I47" s="20"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="23"/>
+      <c r="G48" s="12"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="15"/>
+      <c r="I48" s="20"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="23"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="15"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
+      <c r="A50" s="17"/>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="23"/>
+      <c r="G50" s="12"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="15"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="23"/>
+      <c r="G51" s="12"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="16"/>
+      <c r="I51" s="21"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B52" s="2"/>
@@ -1434,67 +1437,67 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="23"/>
+      <c r="G52" s="12"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="14"/>
+      <c r="I52" s="19"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
+      <c r="A53" s="17"/>
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="23"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="15"/>
+      <c r="I53" s="20"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="23"/>
+      <c r="G54" s="12"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="15"/>
+      <c r="I54" s="20"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="23"/>
+      <c r="G55" s="12"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="15"/>
+      <c r="I55" s="20"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="23"/>
+      <c r="G56" s="12"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="15"/>
+      <c r="I56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="23"/>
+      <c r="G57" s="12"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="16"/>
+      <c r="I57" s="21"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B58" s="2"/>
@@ -1502,89 +1505,89 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="23"/>
+      <c r="G58" s="12"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="14"/>
+      <c r="I58" s="19"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
+      <c r="A59" s="17"/>
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="23"/>
+      <c r="G59" s="12"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="15"/>
+      <c r="I59" s="20"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
+      <c r="A60" s="17"/>
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="23"/>
+      <c r="G60" s="12"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="15"/>
+      <c r="I60" s="20"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
+      <c r="A61" s="17"/>
       <c r="B61" s="2"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="23"/>
+      <c r="G61" s="12"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="15"/>
+      <c r="I61" s="20"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
+      <c r="A62" s="17"/>
       <c r="B62" s="2"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="23"/>
+      <c r="G62" s="12"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="15"/>
+      <c r="I62" s="20"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="2"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="23"/>
+      <c r="G63" s="12"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="15"/>
+      <c r="I63" s="20"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
+      <c r="A64" s="17"/>
       <c r="B64" s="2"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="23"/>
+      <c r="G64" s="12"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="15"/>
+      <c r="I64" s="20"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="2"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="23"/>
+      <c r="G65" s="12"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="16"/>
+      <c r="I65" s="21"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B66" s="2"/>
@@ -1592,56 +1595,56 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="23"/>
+      <c r="G66" s="12"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="14"/>
+      <c r="I66" s="19"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="2"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="23"/>
+      <c r="G67" s="12"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="15"/>
+      <c r="I67" s="20"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="2"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="23"/>
+      <c r="G68" s="12"/>
       <c r="H68" s="1"/>
-      <c r="I68" s="15"/>
+      <c r="I68" s="20"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="2"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="23"/>
+      <c r="G69" s="12"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="15"/>
+      <c r="I69" s="20"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="2"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="23"/>
+      <c r="G70" s="12"/>
       <c r="H70" s="1"/>
-      <c r="I70" s="16"/>
+      <c r="I70" s="21"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B71" s="2"/>
@@ -1649,67 +1652,67 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="23"/>
+      <c r="G71" s="12"/>
       <c r="H71" s="1"/>
-      <c r="I71" s="14"/>
+      <c r="I71" s="19"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
+      <c r="A72" s="17"/>
       <c r="B72" s="2"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="23"/>
+      <c r="G72" s="12"/>
       <c r="H72" s="1"/>
-      <c r="I72" s="15"/>
+      <c r="I72" s="20"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="2"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="23"/>
+      <c r="G73" s="12"/>
       <c r="H73" s="1"/>
-      <c r="I73" s="15"/>
+      <c r="I73" s="20"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
+      <c r="A74" s="17"/>
       <c r="B74" s="2"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="23"/>
+      <c r="G74" s="12"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="15"/>
+      <c r="I74" s="20"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
+      <c r="A75" s="17"/>
       <c r="B75" s="2"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="23"/>
+      <c r="G75" s="12"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="15"/>
+      <c r="I75" s="20"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="2"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="23"/>
+      <c r="G76" s="12"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="16"/>
+      <c r="I76" s="21"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B77" s="2"/>
@@ -1717,78 +1720,78 @@
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="23"/>
+      <c r="G77" s="12"/>
       <c r="H77" s="1"/>
-      <c r="I77" s="14"/>
+      <c r="I77" s="19"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
+      <c r="A78" s="17"/>
       <c r="B78" s="2"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="23"/>
+      <c r="G78" s="12"/>
       <c r="H78" s="1"/>
-      <c r="I78" s="15"/>
+      <c r="I78" s="20"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
+      <c r="A79" s="17"/>
       <c r="B79" s="2"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-      <c r="G79" s="23"/>
+      <c r="G79" s="12"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="15"/>
+      <c r="I79" s="20"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="2"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="23"/>
+      <c r="G80" s="12"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="15"/>
+      <c r="I80" s="20"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="12"/>
+      <c r="A81" s="17"/>
       <c r="B81" s="2"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="23"/>
+      <c r="G81" s="12"/>
       <c r="H81" s="1"/>
-      <c r="I81" s="15"/>
+      <c r="I81" s="20"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="12"/>
+      <c r="A82" s="17"/>
       <c r="B82" s="2"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="23"/>
+      <c r="G82" s="12"/>
       <c r="H82" s="1"/>
-      <c r="I82" s="15"/>
+      <c r="I82" s="20"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="2"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="23"/>
+      <c r="G83" s="12"/>
       <c r="H83" s="1"/>
-      <c r="I83" s="16"/>
+      <c r="I83" s="21"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B84" s="2"/>
@@ -1796,56 +1799,56 @@
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="23"/>
+      <c r="G84" s="12"/>
       <c r="H84" s="1"/>
-      <c r="I84" s="14"/>
+      <c r="I84" s="19"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
+      <c r="A85" s="17"/>
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="23"/>
+      <c r="G85" s="12"/>
       <c r="H85" s="1"/>
-      <c r="I85" s="15"/>
+      <c r="I85" s="20"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
+      <c r="A86" s="17"/>
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="23"/>
+      <c r="G86" s="12"/>
       <c r="H86" s="1"/>
-      <c r="I86" s="15"/>
+      <c r="I86" s="20"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
+      <c r="A87" s="17"/>
       <c r="B87" s="2"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="23"/>
+      <c r="G87" s="12"/>
       <c r="H87" s="1"/>
-      <c r="I87" s="15"/>
+      <c r="I87" s="20"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
+      <c r="A88" s="18"/>
       <c r="B88" s="2"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="23"/>
+      <c r="G88" s="12"/>
       <c r="H88" s="1"/>
-      <c r="I88" s="16"/>
+      <c r="I88" s="21"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B89" s="2"/>
@@ -1853,89 +1856,89 @@
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="23"/>
+      <c r="G89" s="12"/>
       <c r="H89" s="1"/>
-      <c r="I89" s="14"/>
+      <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
+      <c r="A90" s="17"/>
       <c r="B90" s="2"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="23"/>
+      <c r="G90" s="12"/>
       <c r="H90" s="1"/>
-      <c r="I90" s="15"/>
+      <c r="I90" s="20"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
+      <c r="A91" s="17"/>
       <c r="B91" s="2"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="23"/>
+      <c r="G91" s="12"/>
       <c r="H91" s="1"/>
-      <c r="I91" s="15"/>
+      <c r="I91" s="20"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
+      <c r="A92" s="17"/>
       <c r="B92" s="2"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="23"/>
+      <c r="G92" s="12"/>
       <c r="H92" s="1"/>
-      <c r="I92" s="15"/>
+      <c r="I92" s="20"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
+      <c r="A93" s="17"/>
       <c r="B93" s="2"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="23"/>
+      <c r="G93" s="12"/>
       <c r="H93" s="1"/>
-      <c r="I93" s="15"/>
+      <c r="I93" s="20"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
+      <c r="A94" s="17"/>
       <c r="B94" s="2"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-      <c r="G94" s="23"/>
+      <c r="G94" s="12"/>
       <c r="H94" s="1"/>
-      <c r="I94" s="15"/>
+      <c r="I94" s="20"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
+      <c r="A95" s="17"/>
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="23"/>
+      <c r="G95" s="12"/>
       <c r="H95" s="1"/>
-      <c r="I95" s="15"/>
+      <c r="I95" s="20"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
+      <c r="A96" s="18"/>
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-      <c r="G96" s="23"/>
+      <c r="G96" s="12"/>
       <c r="H96" s="1"/>
-      <c r="I96" s="16"/>
+      <c r="I96" s="21"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B97" s="2"/>
@@ -1943,78 +1946,78 @@
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="23"/>
+      <c r="G97" s="12"/>
       <c r="H97" s="1"/>
-      <c r="I97" s="14"/>
+      <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
+      <c r="A98" s="17"/>
       <c r="B98" s="2"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-      <c r="G98" s="23"/>
+      <c r="G98" s="12"/>
       <c r="H98" s="1"/>
-      <c r="I98" s="15"/>
+      <c r="I98" s="20"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
+      <c r="A99" s="17"/>
       <c r="B99" s="2"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="23"/>
+      <c r="G99" s="12"/>
       <c r="H99" s="1"/>
-      <c r="I99" s="15"/>
+      <c r="I99" s="20"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
+      <c r="A100" s="17"/>
       <c r="B100" s="2"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-      <c r="G100" s="23"/>
+      <c r="G100" s="12"/>
       <c r="H100" s="1"/>
-      <c r="I100" s="15"/>
+      <c r="I100" s="20"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
+      <c r="A101" s="17"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
-      <c r="G101" s="23"/>
+      <c r="G101" s="12"/>
       <c r="H101" s="1"/>
-      <c r="I101" s="15"/>
+      <c r="I101" s="20"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
+      <c r="A102" s="17"/>
       <c r="B102" s="2"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
-      <c r="G102" s="23"/>
+      <c r="G102" s="12"/>
       <c r="H102" s="1"/>
-      <c r="I102" s="15"/>
+      <c r="I102" s="20"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="13"/>
+      <c r="A103" s="18"/>
       <c r="B103" s="2"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
-      <c r="G103" s="23"/>
+      <c r="G103" s="12"/>
       <c r="H103" s="1"/>
-      <c r="I103" s="16"/>
+      <c r="I103" s="21"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="14" t="s">
+      <c r="A104" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B104" s="2"/>
@@ -2022,193 +2025,237 @@
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
-      <c r="G104" s="23"/>
+      <c r="G104" s="12"/>
       <c r="H104" s="1"/>
-      <c r="I104" s="14"/>
+      <c r="I104" s="19"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
+      <c r="A105" s="20"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
-      <c r="G105" s="23"/>
+      <c r="G105" s="12"/>
       <c r="H105" s="1"/>
-      <c r="I105" s="15"/>
+      <c r="I105" s="20"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="15"/>
+      <c r="A106" s="20"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
-      <c r="G106" s="23"/>
+      <c r="G106" s="12"/>
       <c r="H106" s="1"/>
-      <c r="I106" s="15"/>
+      <c r="I106" s="20"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="15"/>
+      <c r="A107" s="20"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
-      <c r="G107" s="23"/>
+      <c r="G107" s="12"/>
       <c r="H107" s="1"/>
-      <c r="I107" s="15"/>
+      <c r="I107" s="20"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="20"/>
       <c r="B108" s="2"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
-      <c r="G108" s="23"/>
+      <c r="G108" s="12"/>
       <c r="H108" s="1"/>
-      <c r="I108" s="15"/>
+      <c r="I108" s="20"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="15"/>
+      <c r="A109" s="20"/>
       <c r="B109" s="2"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-      <c r="G109" s="23"/>
+      <c r="G109" s="12"/>
       <c r="H109" s="1"/>
-      <c r="I109" s="15"/>
+      <c r="I109" s="20"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="15"/>
+      <c r="A110" s="20"/>
       <c r="B110" s="2"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
-      <c r="G110" s="23"/>
+      <c r="G110" s="12"/>
       <c r="H110" s="1"/>
-      <c r="I110" s="15"/>
+      <c r="I110" s="20"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="15"/>
+      <c r="A111" s="20"/>
       <c r="B111" s="2"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-      <c r="G111" s="23"/>
+      <c r="G111" s="12"/>
       <c r="H111" s="1"/>
-      <c r="I111" s="15"/>
+      <c r="I111" s="20"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="16"/>
+      <c r="A112" s="21"/>
       <c r="B112" s="2"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
-      <c r="G112" s="23"/>
+      <c r="G112" s="12"/>
       <c r="H112" s="1"/>
-      <c r="I112" s="16"/>
+      <c r="I112" s="21"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C113" s="1"/>
+      <c r="C113" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
-      <c r="G113" s="23"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="11"/>
+      <c r="G113" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I113" s="16" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="15"/>
+      <c r="A114" s="20"/>
       <c r="B114" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C114" s="1"/>
+      <c r="C114" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
-      <c r="G114" s="23"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="12"/>
+      <c r="G114" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I114" s="17"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="15"/>
+      <c r="A115" s="20"/>
       <c r="B115" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C115" s="1"/>
+      <c r="C115" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
-      <c r="G115" s="23"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="12"/>
+      <c r="G115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I115" s="17"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
+      <c r="A116" s="20"/>
       <c r="B116" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C116" s="1"/>
+      <c r="C116" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
-      <c r="G116" s="23"/>
-      <c r="H116" s="1"/>
-      <c r="I116" s="12"/>
+      <c r="G116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I116" s="17"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="15"/>
+      <c r="A117" s="20"/>
       <c r="B117" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C117" s="1"/>
+      <c r="C117" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-      <c r="G117" s="23"/>
-      <c r="H117" s="1"/>
-      <c r="I117" s="12"/>
+      <c r="G117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I117" s="17"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="15"/>
+      <c r="A118" s="20"/>
       <c r="B118" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C118" s="1"/>
+      <c r="C118" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
-      <c r="G118" s="23"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="12"/>
+      <c r="G118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I118" s="17"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="15"/>
+      <c r="A119" s="20"/>
       <c r="B119" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C119" s="1"/>
+      <c r="C119" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
-      <c r="G119" s="23"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="12"/>
+      <c r="G119" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I119" s="17"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="15"/>
+      <c r="A120" s="20"/>
       <c r="B120" s="9" t="s">
         <v>45</v>
       </c>
@@ -2216,12 +2263,12 @@
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
-      <c r="G120" s="23"/>
+      <c r="G120" s="12"/>
       <c r="H120" s="1"/>
-      <c r="I120" s="12"/>
+      <c r="I120" s="17"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="15"/>
+      <c r="A121" s="20"/>
       <c r="B121" s="9" t="s">
         <v>46</v>
       </c>
@@ -2229,12 +2276,12 @@
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
-      <c r="G121" s="23"/>
+      <c r="G121" s="12"/>
       <c r="H121" s="1"/>
-      <c r="I121" s="12"/>
+      <c r="I121" s="17"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="16"/>
+      <c r="A122" s="21"/>
       <c r="B122" s="9" t="s">
         <v>47</v>
       </c>
@@ -2242,9 +2289,9 @@
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
-      <c r="G122" s="23"/>
+      <c r="G122" s="12"/>
       <c r="H122" s="1"/>
-      <c r="I122" s="13"/>
+      <c r="I122" s="18"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
@@ -2255,12 +2302,33 @@
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
-      <c r="G123" s="23"/>
+      <c r="G123" s="12"/>
       <c r="H123" s="1"/>
-      <c r="I123" s="25"/>
+      <c r="I123" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A97:A103"/>
+    <mergeCell ref="A104:A112"/>
+    <mergeCell ref="I16:I25"/>
+    <mergeCell ref="I26:I32"/>
+    <mergeCell ref="I33:I39"/>
+    <mergeCell ref="I40:I44"/>
+    <mergeCell ref="I45:I51"/>
+    <mergeCell ref="I52:I57"/>
+    <mergeCell ref="I58:I65"/>
+    <mergeCell ref="I66:I70"/>
+    <mergeCell ref="I71:I76"/>
+    <mergeCell ref="I77:I83"/>
+    <mergeCell ref="I84:I88"/>
+    <mergeCell ref="I89:I96"/>
+    <mergeCell ref="I97:I103"/>
+    <mergeCell ref="I104:I112"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A89:A96"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I113:I122"/>
     <mergeCell ref="A113:A122"/>
@@ -2277,27 +2345,6 @@
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A57"/>
     <mergeCell ref="A58:A65"/>
-    <mergeCell ref="A66:A70"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A89:A96"/>
-    <mergeCell ref="A97:A103"/>
-    <mergeCell ref="A104:A112"/>
-    <mergeCell ref="I16:I25"/>
-    <mergeCell ref="I26:I32"/>
-    <mergeCell ref="I33:I39"/>
-    <mergeCell ref="I40:I44"/>
-    <mergeCell ref="I45:I51"/>
-    <mergeCell ref="I52:I57"/>
-    <mergeCell ref="I58:I65"/>
-    <mergeCell ref="I66:I70"/>
-    <mergeCell ref="I71:I76"/>
-    <mergeCell ref="I77:I83"/>
-    <mergeCell ref="I84:I88"/>
-    <mergeCell ref="I89:I96"/>
-    <mergeCell ref="I97:I103"/>
-    <mergeCell ref="I104:I112"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
work for recursion ;
Signed-off-by: Aditya Kumar <adikid1996@gmail.com>
</commit_message>
<xml_diff>
--- a/coding-Progress.xlsx
+++ b/coding-Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\go-workspace\src\github.com\aditya109\grokking-the-coding-interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC5AB5B-4358-43D6-95BE-2D2A5DD3F56C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A10F31A-037E-4614-B44C-4C6490BA961A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="251" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14445" yWindow="2580" windowWidth="21600" windowHeight="11385" tabRatio="251" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
   <si>
     <t>Problem Pattern</t>
   </si>
@@ -174,10 +174,25 @@
     <t>Leetcode Run</t>
   </si>
   <si>
-    <t xml:space="preserve">                  </t>
-  </si>
-  <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>equal subset sum partition</t>
+  </si>
+  <si>
+    <t>subset sum</t>
+  </si>
+  <si>
+    <t>minimum subset sum difference</t>
+  </si>
+  <si>
+    <t>count of subset sum</t>
+  </si>
+  <si>
+    <t>target sum</t>
+  </si>
+  <si>
+    <t>number of subsets with diff</t>
   </si>
 </sst>
 </file>
@@ -759,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G125" sqref="G125"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1039,9 @@
       <c r="A16" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1035,7 +1052,9 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1046,8 +1065,8 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="2" t="s">
-        <v>49</v>
+      <c r="B18" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1059,7 +1078,9 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1070,7 +1091,9 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1081,7 +1104,9 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1092,7 +1117,6 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
-      <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2250,7 +2274,7 @@
         <v>33</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I119" s="17"/>
     </row>

</xml_diff>

<commit_message>
added python solution for merge intervals question
Signed-off-by: Aditya Kumar <adikid1996@gmail.com>
</commit_message>
<xml_diff>
--- a/coding-Progress.xlsx
+++ b/coding-Progress.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\MyProjects\Grokking-The-Coding-Interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\aditya109\learning-myself\Grokking-The-Coding-Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA59C7E-F43D-478D-9132-F9D54F8A0303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B6E3B5-4263-43B7-9DAA-B3D3576BE86F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14310" yWindow="4965" windowWidth="21600" windowHeight="11385" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$3:$I$139</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$3:$I$141</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="128">
   <si>
     <t>Problem Pattern</t>
   </si>
@@ -738,6 +738,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,21 +780,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -772,24 +790,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1075,50 +1075,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="6"/>
-    <col min="7" max="7" width="14.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="6"/>
+    <col min="7" max="7" width="14.44140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="28"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
@@ -1134,12 +1134,12 @@
       <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="38"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1155,15 +1155,12 @@
         <v>33</v>
       </c>
       <c r="H3" s="12"/>
-      <c r="I3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="J3" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="36"/>
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1177,13 +1174,10 @@
         <v>33</v>
       </c>
       <c r="H4" s="12"/>
-      <c r="I4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="30"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="36"/>
       <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
@@ -1197,13 +1191,10 @@
         <v>33</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="30"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="36"/>
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
@@ -1217,10 +1208,10 @@
         <v>33</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="J6" s="30"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
       <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
@@ -1234,13 +1225,10 @@
         <v>33</v>
       </c>
       <c r="H7" s="12"/>
-      <c r="I7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="30"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="36"/>
       <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
@@ -1254,10 +1242,10 @@
         <v>33</v>
       </c>
       <c r="H8" s="12"/>
-      <c r="J8" s="30"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="36"/>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
@@ -1271,10 +1259,10 @@
         <v>33</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="J9" s="30"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="36"/>
       <c r="B10" s="9" t="s">
         <v>34</v>
       </c>
@@ -1288,10 +1276,10 @@
         <v>33</v>
       </c>
       <c r="H10" s="12"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="36"/>
       <c r="B11" s="9" t="s">
         <v>35</v>
       </c>
@@ -1305,10 +1293,10 @@
         <v>33</v>
       </c>
       <c r="H11" s="12"/>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="36"/>
       <c r="B12" s="9" t="s">
         <v>36</v>
       </c>
@@ -1318,10 +1306,10 @@
       <c r="F12" s="1"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="36"/>
       <c r="B13" s="9" t="s">
         <v>37</v>
       </c>
@@ -1331,10 +1319,10 @@
       <c r="F13" s="1"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="J13" s="30"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="36"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1342,10 +1330,10 @@
       <c r="F14" s="1"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="J14" s="30"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="37"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1353,10 +1341,10 @@
       <c r="F15" s="1"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1368,10 +1356,10 @@
       <c r="F16" s="1"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="J16" s="29"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
       <c r="B17" s="7" t="s">
         <v>51</v>
       </c>
@@ -1381,10 +1369,10 @@
       <c r="F17" s="1"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="26"/>
       <c r="B18" s="7" t="s">
         <v>52</v>
       </c>
@@ -1394,10 +1382,10 @@
       <c r="F18" s="1"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
       <c r="B19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1407,10 +1395,10 @@
       <c r="F19" s="1"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="J19" s="30"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
       <c r="B20" s="9" t="s">
         <v>53</v>
       </c>
@@ -1420,10 +1408,10 @@
       <c r="F20" s="1"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="J20" s="30"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
       <c r="B21" s="9" t="s">
         <v>54</v>
       </c>
@@ -1433,20 +1421,20 @@
       <c r="F21" s="1"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="J21" s="30"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="J22" s="30"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1454,10 +1442,10 @@
       <c r="F23" s="1"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1465,10 +1453,10 @@
       <c r="F24" s="1"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="J24" s="30"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1476,10 +1464,10 @@
       <c r="F25" s="1"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="J25" s="33"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1495,12 +1483,12 @@
         <v>33</v>
       </c>
       <c r="H26" s="12"/>
-      <c r="J26" s="39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="J26" s="31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
@@ -1514,10 +1502,10 @@
         <v>33</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="J27" s="40"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="J27" s="32"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
       <c r="B28" s="7" t="s">
         <v>58</v>
       </c>
@@ -1527,10 +1515,10 @@
       <c r="F28" s="1"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
-      <c r="J28" s="40"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="41"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1538,10 +1526,10 @@
       <c r="F29" s="1"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
-      <c r="J29" s="40"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1549,10 +1537,10 @@
       <c r="F30" s="1"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
-      <c r="J30" s="40"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1560,10 +1548,10 @@
       <c r="F31" s="1"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
-      <c r="J31" s="40"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="42"/>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1571,10 +1559,10 @@
       <c r="F32" s="1"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
-      <c r="J32" s="41"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="2"/>
@@ -1584,10 +1572,10 @@
       <c r="F33" s="1"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
-      <c r="J33" s="29"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="36"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1595,10 +1583,10 @@
       <c r="F34" s="1"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="J34" s="30"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="J34" s="26"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="36"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1606,10 +1594,10 @@
       <c r="F35" s="1"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="J35" s="30"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="J35" s="26"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="36"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1617,10 +1605,10 @@
       <c r="F36" s="1"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="J36" s="30"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="J36" s="26"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="36"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1628,10 +1616,10 @@
       <c r="F37" s="1"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="J37" s="30"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="J37" s="26"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="36"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1639,10 +1627,10 @@
       <c r="F38" s="1"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
-      <c r="J38" s="30"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="J38" s="26"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="37"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1650,10 +1638,10 @@
       <c r="F39" s="1"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
-      <c r="J39" s="33"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="J39" s="27"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -1671,12 +1659,12 @@
       <c r="H40" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="J40" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="36"/>
       <c r="B41" s="7" t="s">
         <v>60</v>
       </c>
@@ -1692,10 +1680,10 @@
       <c r="H41" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J41" s="30"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="36"/>
       <c r="B42" s="7" t="s">
         <v>61</v>
       </c>
@@ -1711,10 +1699,10 @@
       <c r="H42" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J42" s="30"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="J42" s="26"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="36"/>
       <c r="B43" s="7" t="s">
         <v>62</v>
       </c>
@@ -1730,10 +1718,10 @@
       <c r="H43" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J43" s="30"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="J43" s="26"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="36"/>
       <c r="B44" s="9" t="s">
         <v>63</v>
       </c>
@@ -1749,10 +1737,10 @@
       <c r="H44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J44" s="30"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="J44" s="26"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="36"/>
       <c r="B45" s="9" t="s">
         <v>64</v>
       </c>
@@ -1768,10 +1756,10 @@
       <c r="H45" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J45" s="30"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="J45" s="26"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="36"/>
       <c r="B46" s="9" t="s">
         <v>65</v>
       </c>
@@ -1781,10 +1769,10 @@
       <c r="F46" s="1"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="J46" s="30"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="J46" s="26"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="37"/>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1792,10 +1780,10 @@
       <c r="F47" s="1"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
-      <c r="J47" s="33"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="J47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="35" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="8" t="s">
@@ -1813,10 +1801,10 @@
       <c r="H48" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J48" s="29"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="J48" s="25"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="36"/>
       <c r="B49" s="7" t="s">
         <v>84</v>
       </c>
@@ -1832,10 +1820,10 @@
       <c r="H49" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J49" s="30"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="J49" s="26"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="36"/>
       <c r="B50" s="7" t="s">
         <v>85</v>
       </c>
@@ -1851,10 +1839,10 @@
       <c r="H50" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J50" s="30"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="J50" s="26"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="36"/>
       <c r="B51" s="15" t="s">
         <v>86</v>
       </c>
@@ -1864,10 +1852,10 @@
       <c r="F51" s="1"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
-      <c r="J51" s="30"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="J51" s="26"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="36"/>
       <c r="B52" s="15" t="s">
         <v>87</v>
       </c>
@@ -1877,10 +1865,10 @@
       <c r="F52" s="1"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
-      <c r="J52" s="30"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="J52" s="26"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="36"/>
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1888,10 +1876,10 @@
       <c r="F53" s="1"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
-      <c r="J53" s="30"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
+      <c r="J53" s="26"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="37"/>
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1899,10 +1887,10 @@
       <c r="F54" s="1"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
-      <c r="J54" s="33"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
+      <c r="J54" s="27"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="2"/>
@@ -1912,10 +1900,10 @@
       <c r="F55" s="1"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
-      <c r="J55" s="29"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="J55" s="25"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="36"/>
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1923,10 +1911,10 @@
       <c r="F56" s="1"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
-      <c r="J56" s="30"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="J56" s="26"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="36"/>
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1934,10 +1922,10 @@
       <c r="F57" s="1"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
-      <c r="J57" s="30"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="J57" s="26"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="36"/>
       <c r="B58" s="2"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1945,10 +1933,10 @@
       <c r="F58" s="1"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
-      <c r="J58" s="30"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="J58" s="26"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="36"/>
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1956,10 +1944,10 @@
       <c r="F59" s="1"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
-      <c r="J59" s="30"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
+      <c r="J59" s="26"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="36"/>
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1967,53 +1955,53 @@
       <c r="F60" s="1"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
-      <c r="J60" s="33"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>121</v>
-      </c>
+      <c r="J60" s="26"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="36"/>
+      <c r="B61" s="2"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
-      <c r="J61" s="29"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="42"/>
-      <c r="B62" s="7" t="s">
-        <v>122</v>
-      </c>
+      <c r="J61" s="26"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="37"/>
+      <c r="B62" s="2"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
-      <c r="J62" s="30"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="42"/>
+      <c r="J62" s="27"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="34" t="s">
+        <v>9</v>
+      </c>
       <c r="B63" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C63" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="12"/>
+      <c r="G63" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="H63" s="12"/>
-      <c r="J63" s="30"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="42"/>
+      <c r="J63" s="25"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="34"/>
       <c r="B64" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2021,12 +2009,12 @@
       <c r="F64" s="1"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
-      <c r="J64" s="30"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
-      <c r="B65" s="9" t="s">
-        <v>125</v>
+      <c r="J64" s="26"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="34"/>
+      <c r="B65" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2034,12 +2022,12 @@
       <c r="F65" s="1"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
-      <c r="J65" s="30"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
-      <c r="B66" s="9" t="s">
-        <v>126</v>
+      <c r="J65" s="26"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="34"/>
+      <c r="B66" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2047,12 +2035,12 @@
       <c r="F66" s="1"/>
       <c r="G66" s="12"/>
       <c r="H66" s="12"/>
-      <c r="J66" s="30"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
+      <c r="J66" s="26"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="34"/>
       <c r="B67" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2060,25 +2048,25 @@
       <c r="F67" s="1"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
-      <c r="J67" s="30"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="42"/>
-      <c r="B68" s="2"/>
+      <c r="J67" s="26"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="34"/>
+      <c r="B68" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
-      <c r="J68" s="33"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>99</v>
+      <c r="J68" s="26"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="34"/>
+      <c r="B69" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2086,25 +2074,25 @@
       <c r="F69" s="1"/>
       <c r="G69" s="12"/>
       <c r="H69" s="12"/>
-      <c r="J69" s="29"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
-      <c r="B70" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="J69" s="26"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="34"/>
+      <c r="B70" s="2"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
-      <c r="J70" s="30"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="J70" s="27"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="B71" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2112,12 +2100,12 @@
       <c r="F71" s="1"/>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
-      <c r="J71" s="30"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="J71" s="25"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="36"/>
       <c r="B72" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2125,12 +2113,12 @@
       <c r="F72" s="1"/>
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
-      <c r="J72" s="30"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="26"/>
+      <c r="J72" s="26"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="36"/>
       <c r="B73" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2138,12 +2126,12 @@
       <c r="F73" s="1"/>
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
-      <c r="J73" s="30"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="J73" s="26"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="36"/>
       <c r="B74" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2151,12 +2139,12 @@
       <c r="F74" s="1"/>
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
-      <c r="J74" s="30"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
+      <c r="J74" s="26"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="36"/>
       <c r="B75" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2164,12 +2152,12 @@
       <c r="F75" s="1"/>
       <c r="G75" s="12"/>
       <c r="H75" s="12"/>
-      <c r="J75" s="30"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
-      <c r="B76" s="9" t="s">
-        <v>106</v>
+      <c r="J75" s="26"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="36"/>
+      <c r="B76" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2177,12 +2165,12 @@
       <c r="F76" s="1"/>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
-      <c r="J76" s="30"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
-      <c r="B77" s="9" t="s">
-        <v>107</v>
+      <c r="J76" s="26"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="36"/>
+      <c r="B77" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2190,12 +2178,12 @@
       <c r="F77" s="1"/>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
-      <c r="J77" s="30"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
+      <c r="J77" s="26"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="36"/>
       <c r="B78" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2203,14 +2191,12 @@
       <c r="F78" s="1"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
-      <c r="J78" s="33"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B79" s="21" t="s">
-        <v>11</v>
+      <c r="J78" s="26"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="36"/>
+      <c r="B79" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2218,12 +2204,12 @@
       <c r="F79" s="1"/>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
-      <c r="J79" s="29"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="21" t="s">
-        <v>92</v>
+      <c r="J79" s="26"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="37"/>
+      <c r="B80" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2231,12 +2217,14 @@
       <c r="F80" s="1"/>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
-      <c r="J80" s="30"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
+      <c r="J80" s="27"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="B81" s="21" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2244,12 +2232,12 @@
       <c r="F81" s="1"/>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
-      <c r="J81" s="30"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="J81" s="25"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="36"/>
       <c r="B82" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2257,12 +2245,12 @@
       <c r="F82" s="1"/>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
-      <c r="J82" s="30"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="26"/>
+      <c r="J82" s="26"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="36"/>
       <c r="B83" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2270,12 +2258,12 @@
       <c r="F83" s="1"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
-      <c r="J83" s="30"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
+      <c r="J83" s="26"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="36"/>
       <c r="B84" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2283,12 +2271,12 @@
       <c r="F84" s="1"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
-      <c r="J84" s="30"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="J84" s="26"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="36"/>
       <c r="B85" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2296,12 +2284,12 @@
       <c r="F85" s="1"/>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
-      <c r="J85" s="30"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
-      <c r="B86" s="22" t="s">
-        <v>98</v>
+      <c r="J85" s="26"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="36"/>
+      <c r="B86" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -2309,12 +2297,12 @@
       <c r="F86" s="1"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
-      <c r="J86" s="30"/>
-    </row>
-    <row r="87" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
-      <c r="B87" s="22" t="s">
-        <v>109</v>
+      <c r="J86" s="26"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="36"/>
+      <c r="B87" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -2322,45 +2310,49 @@
       <c r="F87" s="1"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
-      <c r="J87" s="33"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B88" s="2"/>
+      <c r="J87" s="26"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="36"/>
+      <c r="B88" s="22" t="s">
+        <v>98</v>
+      </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
-      <c r="J88" s="29"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
-      <c r="B89" s="2"/>
+      <c r="J88" s="26"/>
+    </row>
+    <row r="89" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="37"/>
+      <c r="B89" s="22" t="s">
+        <v>109</v>
+      </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
-      <c r="J89" s="30"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
-      <c r="B90" s="23"/>
+      <c r="J89" s="27"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="2"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
-      <c r="J90" s="30"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
+      <c r="J90" s="25"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="36"/>
       <c r="B91" s="2"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -2368,21 +2360,21 @@
       <c r="F91" s="1"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
-      <c r="J91" s="30"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="26"/>
-      <c r="B92" s="2"/>
+      <c r="J91" s="26"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="36"/>
+      <c r="B92" s="23"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
-      <c r="J92" s="30"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
+      <c r="J92" s="26"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="36"/>
       <c r="B93" s="2"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -2390,10 +2382,10 @@
       <c r="F93" s="1"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
-      <c r="J93" s="30"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
+      <c r="J93" s="26"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="36"/>
       <c r="B94" s="2"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -2401,61 +2393,55 @@
       <c r="F94" s="1"/>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
-      <c r="J94" s="33"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="J94" s="26"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="36"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H95" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J95" s="29"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
-      <c r="B96" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="J95" s="26"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="37"/>
+      <c r="B96" s="2"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
-      <c r="J96" s="30"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
+      <c r="J96" s="27"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="35" t="s">
+        <v>13</v>
+      </c>
       <c r="B97" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
-      <c r="J97" s="30"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
+      <c r="G97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J97" s="25"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="36"/>
       <c r="B98" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -2463,25 +2449,27 @@
       <c r="F98" s="1"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
-      <c r="J98" s="30"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
+      <c r="J98" s="26"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="36"/>
       <c r="B99" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C99" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
-      <c r="J99" s="30"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
-      <c r="B100" s="9" t="s">
-        <v>116</v>
+      <c r="J99" s="26"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="36"/>
+      <c r="B100" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -2489,12 +2477,12 @@
       <c r="F100" s="1"/>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
-      <c r="J100" s="30"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="27"/>
-      <c r="B101" s="9" t="s">
-        <v>117</v>
+      <c r="J100" s="26"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="36"/>
+      <c r="B101" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -2502,60 +2490,40 @@
       <c r="F101" s="1"/>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
-      <c r="J101" s="33"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="J101" s="26"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="36"/>
+      <c r="B102" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
-      <c r="G102" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H102" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I102" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J102" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
-      <c r="B103" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+      <c r="J102" s="26"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="37"/>
+      <c r="B103" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
-      <c r="G103" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H103" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I103" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J103" s="30"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="26"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="J103" s="27"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="B104" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>33</v>
@@ -2572,12 +2540,14 @@
       <c r="I104" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J104" s="30"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
+      <c r="J104" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="36"/>
       <c r="B105" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>33</v>
@@ -2594,12 +2564,12 @@
       <c r="I105" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J105" s="30"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
+      <c r="J105" s="26"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="36"/>
       <c r="B106" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>33</v>
@@ -2616,12 +2586,12 @@
       <c r="I106" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J106" s="30"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="26"/>
+      <c r="J106" s="26"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="36"/>
       <c r="B107" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>33</v>
@@ -2638,12 +2608,12 @@
       <c r="I107" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J107" s="30"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
-      <c r="B108" s="14" t="s">
-        <v>72</v>
+      <c r="J107" s="26"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="36"/>
+      <c r="B108" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>33</v>
@@ -2660,28 +2630,34 @@
       <c r="I108" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J108" s="30"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
-      <c r="B109" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C109" s="1"/>
+      <c r="J108" s="26"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" s="36"/>
+      <c r="B109" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="12"/>
+      <c r="G109" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H109" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="I109" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J109" s="30"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="27"/>
-      <c r="B110" s="9" t="s">
-        <v>74</v>
+      <c r="J109" s="26"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110" s="36"/>
+      <c r="B110" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>33</v>
@@ -2689,7 +2665,7 @@
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
-      <c r="G110" s="1" t="s">
+      <c r="G110" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H110" s="12" t="s">
@@ -2698,35 +2674,28 @@
       <c r="I110" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J110" s="33"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="J110" s="26"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111" s="36"/>
+      <c r="B111" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-      <c r="G111" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H111" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J111" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
-      <c r="B112" s="7" t="s">
-        <v>76</v>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
+      <c r="I111" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J111" s="26"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112" s="37"/>
+      <c r="B112" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>33</v>
@@ -2740,12 +2709,17 @@
       <c r="H112" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J112" s="30"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="26"/>
+      <c r="I112" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J112" s="27"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" s="35" t="s">
+        <v>15</v>
+      </c>
       <c r="B113" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>33</v>
@@ -2759,12 +2733,14 @@
       <c r="H113" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J113" s="30"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
+      <c r="J113" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="36"/>
       <c r="B114" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>33</v>
@@ -2776,14 +2752,14 @@
         <v>33</v>
       </c>
       <c r="H114" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J114" s="30"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
-      <c r="B115" s="14" t="s">
-        <v>79</v>
+        <v>33</v>
+      </c>
+      <c r="J114" s="26"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" s="36"/>
+      <c r="B115" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>33</v>
@@ -2797,12 +2773,12 @@
       <c r="H115" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J115" s="30"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="26"/>
-      <c r="B116" s="9" t="s">
-        <v>80</v>
+      <c r="J115" s="26"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" s="36"/>
+      <c r="B116" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>33</v>
@@ -2813,41 +2789,51 @@
       <c r="G116" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H116" s="12"/>
-      <c r="J116" s="30"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="27"/>
-      <c r="B117" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C117" s="1"/>
+      <c r="H116" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J116" s="26"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117" s="36"/>
+      <c r="B117" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-      <c r="G117" s="12"/>
-      <c r="H117" s="12"/>
-      <c r="J117" s="33"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C118" s="1"/>
+      <c r="G117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H117" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J117" s="26"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118" s="36"/>
+      <c r="B118" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
-      <c r="G118" s="12"/>
+      <c r="G118" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H118" s="12"/>
-      <c r="J118" s="29"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
-      <c r="B119" s="7" t="s">
-        <v>89</v>
+      <c r="J118" s="26"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119" s="37"/>
+      <c r="B119" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -2855,12 +2841,14 @@
       <c r="F119" s="1"/>
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
-      <c r="J119" s="30"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
+      <c r="J119" s="27"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" s="25" t="s">
+        <v>16</v>
+      </c>
       <c r="B120" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -2868,12 +2856,12 @@
       <c r="F120" s="1"/>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
-      <c r="J120" s="30"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="30"/>
-      <c r="B121" s="9" t="s">
-        <v>91</v>
+      <c r="J120" s="25"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" s="26"/>
+      <c r="B121" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -2881,32 +2869,36 @@
       <c r="F121" s="1"/>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
-      <c r="J121" s="30"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
-      <c r="B122" s="2"/>
+      <c r="J121" s="26"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122" s="26"/>
+      <c r="B122" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="12"/>
       <c r="H122" s="12"/>
-      <c r="J122" s="30"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
-      <c r="B123" s="2"/>
+      <c r="J122" s="26"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" s="26"/>
+      <c r="B123" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
-      <c r="J123" s="30"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="J123" s="26"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" s="26"/>
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2914,10 +2906,10 @@
       <c r="F124" s="1"/>
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
-      <c r="J124" s="30"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="30"/>
+      <c r="J124" s="26"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" s="26"/>
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -2925,10 +2917,10 @@
       <c r="F125" s="1"/>
       <c r="G125" s="12"/>
       <c r="H125" s="12"/>
-      <c r="J125" s="30"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="33"/>
+      <c r="J125" s="26"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" s="26"/>
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -2936,53 +2928,35 @@
       <c r="F126" s="1"/>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
-      <c r="J126" s="33"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" s="29" t="s">
-        <v>17</v>
-      </c>
+      <c r="J126" s="26"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A127" s="26"/>
       <c r="B127" s="2"/>
-      <c r="C127" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
-      <c r="G127" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H127" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J127" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" s="30"/>
-      <c r="B128" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
+      <c r="J127" s="26"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" s="27"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
-      <c r="G128" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H128" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J128" s="30"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
-      <c r="B129" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="G128" s="12"/>
+      <c r="H128" s="12"/>
+      <c r="J128" s="27"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" s="2"/>
       <c r="C129" s="1" t="s">
         <v>33</v>
       </c>
@@ -2995,12 +2969,14 @@
       <c r="H129" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J129" s="30"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="J129" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A130" s="26"/>
       <c r="B130" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>33</v>
@@ -3014,12 +2990,12 @@
       <c r="H130" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J130" s="30"/>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="J130" s="26"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A131" s="26"/>
       <c r="B131" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>33</v>
@@ -3033,12 +3009,12 @@
       <c r="H131" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J131" s="30"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A132" s="30"/>
+      <c r="J131" s="26"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A132" s="26"/>
       <c r="B132" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>33</v>
@@ -3052,12 +3028,12 @@
       <c r="H132" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J132" s="30"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="J132" s="26"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A133" s="26"/>
       <c r="B133" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>33</v>
@@ -3069,81 +3045,93 @@
         <v>33</v>
       </c>
       <c r="H133" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J133" s="30"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="J133" s="26"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A134" s="26"/>
       <c r="B134" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C134" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-      <c r="J134" s="30"/>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" s="30"/>
-      <c r="B135" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C135" s="1"/>
+      <c r="G134" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H134" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J134" s="26"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A135" s="26"/>
+      <c r="B135" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
-      <c r="G135" s="12"/>
-      <c r="H135" s="12"/>
-      <c r="J135" s="30"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" s="30"/>
-      <c r="B136" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C136" s="16"/>
-      <c r="D136" s="16"/>
-      <c r="E136" s="16"/>
-      <c r="F136" s="16"/>
-      <c r="G136" s="19"/>
-      <c r="H136" s="19"/>
-      <c r="J136" s="33"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B137" s="20" t="s">
-        <v>118</v>
+      <c r="G135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H135" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J135" s="26"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A136" s="26"/>
+      <c r="B136" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="12"/>
+      <c r="J136" s="26"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A137" s="26"/>
+      <c r="B137" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
-      <c r="G137" s="1"/>
+      <c r="G137" s="12"/>
       <c r="H137" s="12"/>
-      <c r="J137" s="24"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J137" s="26"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="26"/>
-      <c r="B138" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C138" s="1"/>
-      <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
-      <c r="F138" s="1"/>
-      <c r="G138" s="1"/>
-      <c r="H138" s="12"/>
-      <c r="J138" s="24"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" s="27"/>
+      <c r="B138" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C138" s="16"/>
+      <c r="D138" s="16"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="19"/>
+      <c r="H138" s="19"/>
+      <c r="J138" s="27"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A139" s="35" t="s">
+        <v>18</v>
+      </c>
       <c r="B139" s="20" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -3153,37 +3141,40 @@
       <c r="H139" s="12"/>
       <c r="J139" s="24"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B140" s="18"/>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A140" s="36"/>
+      <c r="B140" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="12"/>
+      <c r="J140" s="24"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A141" s="37"/>
+      <c r="B141" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="12"/>
+      <c r="J141" s="24"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B142" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="J16:J25"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J118:J126"/>
-    <mergeCell ref="J3:J15"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="J79:J87"/>
-    <mergeCell ref="J69:J78"/>
-    <mergeCell ref="J61:J68"/>
-    <mergeCell ref="J55:J60"/>
-    <mergeCell ref="J48:J54"/>
-    <mergeCell ref="J40:J47"/>
-    <mergeCell ref="J33:J39"/>
-    <mergeCell ref="J26:J32"/>
-    <mergeCell ref="J127:J136"/>
-    <mergeCell ref="J111:J117"/>
-    <mergeCell ref="J102:J110"/>
-    <mergeCell ref="J95:J101"/>
-    <mergeCell ref="J88:J94"/>
-    <mergeCell ref="A61:A68"/>
-    <mergeCell ref="A69:A78"/>
-    <mergeCell ref="A79:A87"/>
-    <mergeCell ref="A88:A94"/>
-    <mergeCell ref="A95:A101"/>
-    <mergeCell ref="A137:A139"/>
+    <mergeCell ref="A139:A141"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A127:A136"/>
+    <mergeCell ref="A129:A138"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -3193,10 +3184,33 @@
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A102:A110"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A118:A126"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="A104:A112"/>
+    <mergeCell ref="A113:A119"/>
+    <mergeCell ref="A120:A128"/>
+    <mergeCell ref="A63:A70"/>
+    <mergeCell ref="A71:A80"/>
+    <mergeCell ref="A81:A89"/>
+    <mergeCell ref="A90:A96"/>
+    <mergeCell ref="A97:A103"/>
+    <mergeCell ref="J129:J138"/>
+    <mergeCell ref="J113:J119"/>
+    <mergeCell ref="J104:J112"/>
+    <mergeCell ref="J97:J103"/>
+    <mergeCell ref="J90:J96"/>
+    <mergeCell ref="J16:J25"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J120:J128"/>
+    <mergeCell ref="J3:J15"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="J81:J89"/>
+    <mergeCell ref="J71:J80"/>
+    <mergeCell ref="J63:J70"/>
+    <mergeCell ref="J55:J62"/>
+    <mergeCell ref="J48:J54"/>
+    <mergeCell ref="J40:J47"/>
+    <mergeCell ref="J33:J39"/>
+    <mergeCell ref="J26:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>